<commit_message>
DSP çalışıyor !!!11!1bir. @furkankarakaya, @ozank DSP'ye bağlanıldı, kod atıldı, debug edildi. Enable kullanılarak LED yakıp söndürüldü. Special thanx to @hakansrc.
</commit_message>
<xml_diff>
--- a/Prototype/Test/kontrol kartı/Kontrol Kartı Test Planı.xlsx
+++ b/Prototype/Test/kontrol kartı/Kontrol Kartı Test Planı.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="577">
   <si>
     <t>Test Türü</t>
   </si>
@@ -2631,9 +2631,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H349" sqref="H349"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A332" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H356" sqref="H356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2642,9 +2642,9 @@
     <col min="2" max="2" width="31" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="6" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" style="6" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" style="6" customWidth="1"/>
     <col min="10" max="10" width="36.7109375" style="17" customWidth="1"/>
@@ -11265,98 +11265,108 @@
         <v>328</v>
       </c>
       <c r="B348" s="51"/>
-      <c r="C348" s="33" t="s">
+      <c r="C348" s="47" t="s">
         <v>466</v>
       </c>
-      <c r="D348" s="5" t="s">
+      <c r="D348" s="29" t="s">
         <v>482</v>
       </c>
-      <c r="E348" s="33" t="s">
+      <c r="E348" s="47" t="s">
         <v>512</v>
       </c>
-      <c r="F348" s="33" t="s">
+      <c r="F348" s="47" t="s">
         <v>469</v>
       </c>
-      <c r="G348" s="36" t="s">
+      <c r="G348" s="39" t="s">
         <v>508</v>
       </c>
-      <c r="H348" s="5" t="s">
+      <c r="H348" s="29" t="s">
         <v>509</v>
       </c>
-      <c r="I348" s="5"/>
-      <c r="J348" s="15"/>
+      <c r="I348" s="29" t="s">
+        <v>518</v>
+      </c>
+      <c r="J348" s="14"/>
     </row>
     <row r="349" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A349" s="8">
         <v>329</v>
       </c>
       <c r="B349" s="51"/>
-      <c r="C349" s="34"/>
-      <c r="D349" s="5" t="s">
+      <c r="C349" s="49"/>
+      <c r="D349" s="29" t="s">
         <v>483</v>
       </c>
-      <c r="E349" s="34"/>
-      <c r="F349" s="34"/>
-      <c r="G349" s="37"/>
-      <c r="H349" s="5" t="s">
+      <c r="E349" s="49"/>
+      <c r="F349" s="49"/>
+      <c r="G349" s="40"/>
+      <c r="H349" s="29" t="s">
         <v>510</v>
       </c>
-      <c r="I349" s="5"/>
-      <c r="J349" s="15"/>
+      <c r="I349" s="29" t="s">
+        <v>518</v>
+      </c>
+      <c r="J349" s="14"/>
     </row>
     <row r="350" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A350" s="8">
         <v>330</v>
       </c>
       <c r="B350" s="51"/>
-      <c r="C350" s="34"/>
-      <c r="D350" s="5" t="s">
+      <c r="C350" s="49"/>
+      <c r="D350" s="29" t="s">
         <v>484</v>
       </c>
-      <c r="E350" s="34"/>
-      <c r="F350" s="34"/>
-      <c r="G350" s="37"/>
-      <c r="H350" s="5" t="s">
+      <c r="E350" s="49"/>
+      <c r="F350" s="49"/>
+      <c r="G350" s="40"/>
+      <c r="H350" s="29" t="s">
         <v>511</v>
       </c>
-      <c r="I350" s="5"/>
-      <c r="J350" s="15"/>
+      <c r="I350" s="29" t="s">
+        <v>518</v>
+      </c>
+      <c r="J350" s="14"/>
     </row>
     <row r="351" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A351" s="8">
         <v>331</v>
       </c>
       <c r="B351" s="51"/>
-      <c r="C351" s="34"/>
-      <c r="D351" s="5" t="s">
+      <c r="C351" s="49"/>
+      <c r="D351" s="29" t="s">
         <v>513</v>
       </c>
-      <c r="E351" s="34"/>
-      <c r="F351" s="34"/>
-      <c r="G351" s="37"/>
-      <c r="H351" s="5" t="s">
+      <c r="E351" s="49"/>
+      <c r="F351" s="49"/>
+      <c r="G351" s="40"/>
+      <c r="H351" s="29" t="s">
         <v>510</v>
       </c>
-      <c r="I351" s="5"/>
-      <c r="J351" s="15"/>
+      <c r="I351" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="J351" s="14"/>
     </row>
     <row r="352" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A352" s="8">
         <v>332</v>
       </c>
       <c r="B352" s="52"/>
-      <c r="C352" s="35"/>
-      <c r="D352" s="5" t="s">
+      <c r="C352" s="48"/>
+      <c r="D352" s="29" t="s">
         <v>514</v>
       </c>
-      <c r="E352" s="35"/>
-      <c r="F352" s="35"/>
-      <c r="G352" s="38"/>
-      <c r="H352" s="5" t="s">
+      <c r="E352" s="48"/>
+      <c r="F352" s="48"/>
+      <c r="G352" s="41"/>
+      <c r="H352" s="29" t="s">
         <v>515</v>
       </c>
-      <c r="I352" s="5"/>
-      <c r="J352" s="15"/>
+      <c r="I352" s="29" t="s">
+        <v>518</v>
+      </c>
+      <c r="J352" s="14"/>
     </row>
     <row r="353" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A353" s="30" t="s">

</xml_diff>